<commit_message>
revise supply chain base
</commit_message>
<xml_diff>
--- a/MP/SupplyChain/test.xlsx
+++ b/MP/SupplyChain/test.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plants" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Customers" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Products" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ProductionCosts" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Demand" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TransportationCosts" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="ProductionCapacity" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="ProductionPlan" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="TransportationPlan" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Delivery" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Plants" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Customers" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Products" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductionCosts" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Demand" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TransportationCosts" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductionCapacity" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ProductionPlan" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TransportationPlan" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Delivery" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1421,7 +1421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1432,25 +1432,30 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>ProductName</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>PlantName</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>CustomerName</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>X_transportation</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>X_transportation_Solution</t>
         </is>
@@ -1460,27 +1465,30 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Product1</t>
-        </is>
+      <c r="B2" t="n">
+        <v>0</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Product1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Plant1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>Customer1</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>X_transportation_Product1_Plant1_Customer1</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1488,27 +1496,30 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Product1</t>
-        </is>
+      <c r="B3" t="n">
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Product1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Plant1</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Customer2</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>X_transportation_Product1_Plant1_Customer2</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>500</v>
       </c>
     </row>
@@ -1516,27 +1527,30 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Product1</t>
-        </is>
+      <c r="B4" t="n">
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Product1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Plant2</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Customer1</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>X_transportation_Product1_Plant2_Customer1</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>200</v>
       </c>
     </row>
@@ -1544,27 +1558,30 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Product1</t>
-        </is>
+      <c r="B5" t="n">
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Product1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Plant2</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Customer2</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>X_transportation_Product1_Plant2_Customer2</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1572,27 +1589,30 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Product2</t>
-        </is>
+      <c r="B6" t="n">
+        <v>4</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Product2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Plant1</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Customer1</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>X_transportation_Product2_Plant1_Customer1</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1600,27 +1620,30 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Product2</t>
-        </is>
+      <c r="B7" t="n">
+        <v>5</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Product2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Plant1</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Customer2</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>X_transportation_Product2_Plant1_Customer2</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>300</v>
       </c>
     </row>
@@ -1628,27 +1651,30 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Product2</t>
-        </is>
+      <c r="B8" t="n">
+        <v>6</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Product2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Plant2</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Customer1</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>X_transportation_Product2_Plant2_Customer1</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>300</v>
       </c>
     </row>
@@ -1656,27 +1682,30 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Product2</t>
-        </is>
+      <c r="B9" t="n">
+        <v>7</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Product2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>Plant2</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Customer2</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>X_transportation_Product2_Plant2_Customer2</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>